<commit_message>
improved occupancy, added ticket sales
</commit_message>
<xml_diff>
--- a/Track Layout & Vehicle Data vF2.xlsx
+++ b/Track Layout & Vehicle Data vF2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshuttleworth/Desktop/ECE 1140/trains/ECE1140/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8460D32-93D5-2D4E-9872-542B2F7AAA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8789E3-8E39-214E-B674-8396085624C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="32620" windowHeight="20500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -170,25 +170,16 @@
     <t>UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; PENN STATION; UNDERGROUND</t>
-  </si>
-  <si>
     <t>SWITCH (27-28; 27-76); UNDERGROUND</t>
   </si>
   <si>
     <t>SWITCH (33-32; 33-72); UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION;     STEEL PLAZA; UNDERGROUND</t>
-  </si>
-  <si>
     <t>SWITCH (38-39; 38-71); UNDERGROUND</t>
   </si>
   <si>
     <t>SWITCH (44-43, 44-67); UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; FIRST AVE; UNDERGROUND</t>
   </si>
   <si>
     <t>I</t>
@@ -340,6 +331,15 @@
   <si>
     <t xml:space="preserve">UNDERGROUND; STATION; OVERBROOK; </t>
   </si>
+  <si>
+    <t>UNDERGROUND; STATION; PENN STATION</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; STATION; STEEL PLAZA</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; STATION; FIRST AVE</t>
+  </si>
 </sst>
 </file>
 
@@ -350,9 +350,16 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -467,30 +474,30 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -499,53 +506,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2256,9 +2269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2311,7 +2324,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -2582,7 +2595,7 @@
       <c r="F9" s="13">
         <v>40</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="33" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="13" t="s">
@@ -2962,7 +2975,7 @@
       <c r="F19" s="13">
         <v>55</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="33" t="s">
         <v>37</v>
       </c>
       <c r="H19" s="13" t="s">
@@ -3107,7 +3120,7 @@
       <c r="F23" s="13">
         <v>55</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="33" t="s">
         <v>39</v>
       </c>
       <c r="H23" s="13" t="s">
@@ -3253,8 +3266,8 @@
       <c r="F27" s="13">
         <v>70</v>
       </c>
-      <c r="G27" s="19" t="s">
-        <v>42</v>
+      <c r="G27" s="33" t="s">
+        <v>96</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>28</v>
@@ -3330,7 +3343,7 @@
         <v>70</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="25">
@@ -3552,7 +3565,7 @@
         <v>70</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="25">
@@ -3625,8 +3638,8 @@
       <c r="F37" s="13">
         <v>70</v>
       </c>
-      <c r="G37" s="19" t="s">
-        <v>45</v>
+      <c r="G37" s="33" t="s">
+        <v>97</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>28</v>
@@ -3739,7 +3752,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="25">
@@ -3961,7 +3974,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="25">
@@ -3997,8 +4010,8 @@
       <c r="F47" s="13">
         <v>70</v>
       </c>
-      <c r="G47" s="19" t="s">
-        <v>48</v>
+      <c r="G47" s="33" t="s">
+        <v>98</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>28</v>
@@ -4022,7 +4035,7 @@
         <v>Red</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C48" s="13">
         <v>46</v>
@@ -4059,7 +4072,7 @@
         <v>Red</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C49" s="24">
         <v>47</v>
@@ -4074,7 +4087,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="25">
@@ -4096,7 +4109,7 @@
         <v>Red</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C50" s="13">
         <v>48</v>
@@ -4111,7 +4124,7 @@
         <v>70</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>28</v>
@@ -4135,7 +4148,7 @@
         <v>Red</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C51" s="13">
         <v>49</v>
@@ -4170,7 +4183,7 @@
         <v>Red</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C52" s="24">
         <v>50</v>
@@ -4205,7 +4218,7 @@
         <v>Red</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C53" s="13">
         <v>51</v>
@@ -4240,7 +4253,7 @@
         <v>Red</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C54" s="13">
         <v>52</v>
@@ -4255,7 +4268,7 @@
         <v>55</v>
       </c>
       <c r="G54" s="21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H54" s="13"/>
       <c r="I54" s="25">
@@ -4277,7 +4290,7 @@
         <v>Red</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C55" s="24">
         <v>53</v>
@@ -4312,7 +4325,7 @@
         <v>Red</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C56" s="13">
         <v>54</v>
@@ -4347,7 +4360,7 @@
         <v>Red</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C57" s="13">
         <v>55</v>
@@ -4382,7 +4395,7 @@
         <v>Red</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C58" s="24">
         <v>56</v>
@@ -4417,7 +4430,7 @@
         <v>Red</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C59" s="13">
         <v>57</v>
@@ -4452,7 +4465,7 @@
         <v>Red</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C60" s="13">
         <v>58</v>
@@ -4487,7 +4500,7 @@
         <v>Red</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C61" s="24">
         <v>59</v>
@@ -4522,7 +4535,7 @@
         <v>Red</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C62" s="13">
         <v>60</v>
@@ -4537,7 +4550,7 @@
         <v>55</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H62" s="13" t="s">
         <v>28</v>
@@ -4561,7 +4574,7 @@
         <v>Red</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C63" s="13">
         <v>61</v>
@@ -4596,7 +4609,7 @@
         <v>Red</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C64" s="24">
         <v>62</v>
@@ -4631,7 +4644,7 @@
         <v>Red</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C65" s="13">
         <v>63</v>
@@ -4666,7 +4679,7 @@
         <v>Red</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C66" s="13">
         <v>64</v>
@@ -4701,7 +4714,7 @@
         <v>Red</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C67" s="24">
         <v>65</v>
@@ -4736,7 +4749,7 @@
         <v>Red</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C68" s="13">
         <v>66</v>
@@ -4771,7 +4784,7 @@
         <v>Red</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C69" s="13">
         <v>67</v>
@@ -4808,7 +4821,7 @@
         <v>Red</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C70" s="24">
         <v>68</v>
@@ -4845,7 +4858,7 @@
         <v>Red</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C71" s="13">
         <v>69</v>
@@ -4882,7 +4895,7 @@
         <v>Red</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C72" s="13">
         <v>70</v>
@@ -4919,7 +4932,7 @@
         <v>Red</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C73" s="24">
         <v>71</v>
@@ -4956,7 +4969,7 @@
         <v>Red</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C74" s="13">
         <v>72</v>
@@ -4993,7 +5006,7 @@
         <v>Red</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C75" s="13">
         <v>73</v>
@@ -5030,7 +5043,7 @@
         <v>Red</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C76" s="24">
         <v>74</v>
@@ -5067,7 +5080,7 @@
         <v>Red</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C77" s="13">
         <v>75</v>
@@ -5104,7 +5117,7 @@
         <v>Red</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C78" s="13">
         <v>76</v>
@@ -5137,7 +5150,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="24"/>
@@ -5164,15 +5177,16 @@
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B81" s="13"/>
       <c r="C81" s="24"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" s="34"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5180,7 +5194,7 @@
       <c r="B82" s="13"/>
       <c r="C82" s="24"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5188,7 +5202,7 @@
       <c r="B83" s="13"/>
       <c r="C83" s="24"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5196,7 +5210,7 @@
       <c r="B84" s="13"/>
       <c r="C84" s="24"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5204,7 +5218,7 @@
       <c r="B85" s="13"/>
       <c r="C85" s="24"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5212,7 +5226,7 @@
       <c r="B86" s="13"/>
       <c r="C86" s="24"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5220,7 +5234,7 @@
       <c r="B87" s="13"/>
       <c r="C87" s="24"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5228,7 +5242,7 @@
       <c r="B88" s="13"/>
       <c r="C88" s="24"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5236,7 +5250,7 @@
       <c r="B89" s="13"/>
       <c r="C89" s="24"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5244,7 +5258,7 @@
       <c r="B90" s="13"/>
       <c r="C90" s="24"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5252,7 +5266,7 @@
       <c r="B91" s="13"/>
       <c r="C91" s="24"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5260,7 +5274,7 @@
       <c r="B92" s="13"/>
       <c r="C92" s="24"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5268,7 +5282,7 @@
       <c r="B93" s="13"/>
       <c r="C93" s="24"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5276,7 +5290,7 @@
       <c r="B94" s="13"/>
       <c r="C94" s="24"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5284,7 +5298,7 @@
       <c r="B95" s="13"/>
       <c r="C95" s="24"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5774,9 +5788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G145" sqref="G145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5826,7 +5840,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -5843,7 +5857,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="6"/>
@@ -5854,7 +5868,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>13</v>
@@ -5909,10 +5923,10 @@
         <v>45</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I4" s="13">
         <f t="shared" ref="I4:I67" si="0">E4*D4/100</f>
@@ -6178,10 +6192,10 @@
         <v>45</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="0"/>
@@ -6334,7 +6348,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13">
@@ -6445,7 +6459,7 @@
         <v>70</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>28</v>
@@ -6554,7 +6568,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13">
@@ -6661,7 +6675,7 @@
         <v>70</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>28</v>
@@ -6875,7 +6889,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13">
@@ -6982,10 +6996,10 @@
         <v>30</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I33" s="13">
         <f t="shared" si="0"/>
@@ -7146,7 +7160,7 @@
         <v>Green</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C38" s="13">
         <v>36</v>
@@ -7183,7 +7197,7 @@
         <v>Green</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C39" s="13">
         <v>37</v>
@@ -7220,7 +7234,7 @@
         <v>Green</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C40" s="24">
         <v>38</v>
@@ -7257,7 +7271,7 @@
         <v>Green</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41" s="13">
         <v>39</v>
@@ -7271,11 +7285,11 @@
       <c r="F41" s="13">
         <v>30</v>
       </c>
-      <c r="G41" s="32" t="s">
-        <v>96</v>
+      <c r="G41" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I41" s="13">
         <f t="shared" si="0"/>
@@ -7296,7 +7310,7 @@
         <v>Green</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C42" s="13">
         <v>40</v>
@@ -7333,7 +7347,7 @@
         <v>Green</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" s="24">
         <v>41</v>
@@ -7370,7 +7384,7 @@
         <v>Green</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C44" s="13">
         <v>42</v>
@@ -7407,7 +7421,7 @@
         <v>Green</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C45" s="13">
         <v>43</v>
@@ -7444,7 +7458,7 @@
         <v>Green</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C46" s="24">
         <v>44</v>
@@ -7481,7 +7495,7 @@
         <v>Green</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C47" s="13">
         <v>45</v>
@@ -7518,7 +7532,7 @@
         <v>Green</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C48" s="13">
         <v>46</v>
@@ -7555,7 +7569,7 @@
         <v>Green</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C49" s="24">
         <v>47</v>
@@ -7592,7 +7606,7 @@
         <v>Green</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C50" s="13">
         <v>48</v>
@@ -7606,11 +7620,11 @@
       <c r="F50" s="13">
         <v>30</v>
       </c>
-      <c r="G50" s="32" t="s">
-        <v>97</v>
+      <c r="G50" s="30" t="s">
+        <v>94</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I50" s="13">
         <f t="shared" si="0"/>
@@ -7631,7 +7645,7 @@
         <v>Green</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C51" s="13">
         <v>49</v>
@@ -7668,7 +7682,7 @@
         <v>Green</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C52" s="24">
         <v>50</v>
@@ -7705,7 +7719,7 @@
         <v>Green</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C53" s="13">
         <v>51</v>
@@ -7742,7 +7756,7 @@
         <v>Green</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C54" s="13">
         <v>52</v>
@@ -7779,7 +7793,7 @@
         <v>Green</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C55" s="24">
         <v>53</v>
@@ -7816,7 +7830,7 @@
         <v>Green</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C56" s="13">
         <v>54</v>
@@ -7853,7 +7867,7 @@
         <v>Green</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C57" s="13">
         <v>55</v>
@@ -7890,7 +7904,7 @@
         <v>Green</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C58" s="24">
         <v>56</v>
@@ -7904,8 +7918,8 @@
       <c r="F58" s="13">
         <v>30</v>
       </c>
-      <c r="G58" s="32" t="s">
-        <v>98</v>
+      <c r="G58" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="H58" s="13"/>
       <c r="I58" s="13">
@@ -7927,7 +7941,7 @@
         <v>Green</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C59" s="13">
         <v>57</v>
@@ -7942,10 +7956,10 @@
         <v>30</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I59" s="13">
         <f t="shared" si="0"/>
@@ -7966,7 +7980,7 @@
         <v>Green</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C60" s="13">
         <v>58</v>
@@ -8001,7 +8015,7 @@
         <v>Green</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C61" s="24">
         <v>59</v>
@@ -8036,7 +8050,7 @@
         <v>Green</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C62" s="13">
         <v>60</v>
@@ -8071,7 +8085,7 @@
         <v>Green</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C63" s="13">
         <v>61</v>
@@ -8106,7 +8120,7 @@
         <v>Green</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C64" s="24">
         <v>62</v>
@@ -8141,7 +8155,7 @@
         <v>Green</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C65" s="13">
         <v>63</v>
@@ -8156,7 +8170,7 @@
         <v>70</v>
       </c>
       <c r="G65" s="21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H65" s="13"/>
       <c r="I65" s="13">
@@ -8178,7 +8192,7 @@
         <v>Green</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C66" s="13">
         <v>64</v>
@@ -8213,7 +8227,7 @@
         <v>Green</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C67" s="24">
         <v>65</v>
@@ -8228,10 +8242,10 @@
         <v>70</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I67" s="13">
         <f t="shared" si="0"/>
@@ -8252,7 +8266,7 @@
         <v>Green</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C68" s="13">
         <v>66</v>
@@ -8287,7 +8301,7 @@
         <v>Green</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C69" s="13">
         <v>67</v>
@@ -8322,7 +8336,7 @@
         <v>Green</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C70" s="24">
         <v>68</v>
@@ -8357,7 +8371,7 @@
         <v>Green</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C71" s="13">
         <v>69</v>
@@ -8392,7 +8406,7 @@
         <v>Green</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C72" s="13">
         <v>70</v>
@@ -8427,7 +8441,7 @@
         <v>Green</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C73" s="24">
         <v>71</v>
@@ -8462,7 +8476,7 @@
         <v>Green</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C74" s="13">
         <v>72</v>
@@ -8497,7 +8511,7 @@
         <v>Green</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C75" s="13">
         <v>73</v>
@@ -8512,10 +8526,10 @@
         <v>40</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I75" s="13">
         <f t="shared" si="5"/>
@@ -8536,7 +8550,7 @@
         <v>Green</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C76" s="24">
         <v>74</v>
@@ -8571,7 +8585,7 @@
         <v>Green</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C77" s="13">
         <v>75</v>
@@ -8606,7 +8620,7 @@
         <v>Green</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C78" s="13">
         <v>76</v>
@@ -8641,7 +8655,7 @@
         <v>Green</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C79" s="13">
         <v>77</v>
@@ -8656,7 +8670,7 @@
         <v>70</v>
       </c>
       <c r="G79" s="21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H79" s="13"/>
       <c r="I79" s="13">
@@ -8678,7 +8692,7 @@
         <v>Green</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C80" s="24">
         <v>78</v>
@@ -8693,7 +8707,7 @@
         <v>70</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H80" s="13" t="s">
         <v>28</v>
@@ -8717,7 +8731,7 @@
         <v>Green</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C81" s="13">
         <v>79</v>
@@ -8752,7 +8766,7 @@
         <v>Green</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C82" s="13">
         <v>80</v>
@@ -8787,7 +8801,7 @@
         <v>Green</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C83" s="13">
         <v>81</v>
@@ -8822,7 +8836,7 @@
         <v>Green</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C84" s="24">
         <v>82</v>
@@ -8857,7 +8871,7 @@
         <v>Green</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C85" s="13">
         <v>83</v>
@@ -8892,7 +8906,7 @@
         <v>Green</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C86" s="13">
         <v>84</v>
@@ -8927,7 +8941,7 @@
         <v>Green</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C87" s="13">
         <v>85</v>
@@ -8942,7 +8956,7 @@
         <v>70</v>
       </c>
       <c r="G87" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="13">
@@ -8964,7 +8978,7 @@
         <v>Green</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C88" s="24">
         <v>86</v>
@@ -8999,7 +9013,7 @@
         <v>Green</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C89" s="13">
         <v>87</v>
@@ -9034,7 +9048,7 @@
         <v>Green</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C90" s="13">
         <v>88</v>
@@ -9049,10 +9063,10 @@
         <v>25</v>
       </c>
       <c r="G90" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I90" s="13">
         <f t="shared" si="8"/>
@@ -9073,7 +9087,7 @@
         <v>Green</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C91" s="13">
         <v>89</v>
@@ -9108,7 +9122,7 @@
         <v>Green</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C92" s="24">
         <v>90</v>
@@ -9143,7 +9157,7 @@
         <v>Green</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C93" s="13">
         <v>91</v>
@@ -9178,7 +9192,7 @@
         <v>Green</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C94" s="13">
         <v>92</v>
@@ -9213,7 +9227,7 @@
         <v>Green</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C95" s="13">
         <v>93</v>
@@ -9248,7 +9262,7 @@
         <v>Green</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C96" s="24">
         <v>94</v>
@@ -9283,7 +9297,7 @@
         <v>Green</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C97" s="13">
         <v>95</v>
@@ -9318,7 +9332,7 @@
         <v>Green</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C98" s="13">
         <v>96</v>
@@ -9333,10 +9347,10 @@
         <v>25</v>
       </c>
       <c r="G98" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I98" s="13">
         <f t="shared" si="8"/>
@@ -9357,7 +9371,7 @@
         <v>Green</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C99" s="13">
         <v>97</v>
@@ -9392,7 +9406,7 @@
         <v>Green</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C100" s="24">
         <v>98</v>
@@ -9427,7 +9441,7 @@
         <v>Green</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C101" s="13">
         <v>99</v>
@@ -9462,7 +9476,7 @@
         <v>Green</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C102" s="13">
         <v>100</v>
@@ -9497,7 +9511,7 @@
         <v>Green</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C103" s="13">
         <v>101</v>
@@ -9532,7 +9546,7 @@
         <v>Green</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C104" s="24">
         <v>102</v>
@@ -9567,7 +9581,7 @@
         <v>Green</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C105" s="13">
         <v>103</v>
@@ -9602,7 +9616,7 @@
         <v>Green</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C106" s="13">
         <v>104</v>
@@ -9637,7 +9651,7 @@
         <v>Green</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C107" s="13">
         <v>105</v>
@@ -9656,7 +9670,7 @@
         <v>STATION; DORMONT</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I107" s="13">
         <f t="shared" si="8"/>
@@ -9677,7 +9691,7 @@
         <v>Green</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C108" s="24">
         <v>106</v>
@@ -9712,7 +9726,7 @@
         <v>Green</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C109" s="13">
         <v>107</v>
@@ -9747,7 +9761,7 @@
         <v>Green</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C110" s="13">
         <v>108</v>
@@ -9782,7 +9796,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C111" s="13">
         <v>109</v>
@@ -9817,7 +9831,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C112" s="24">
         <v>110</v>
@@ -9852,7 +9866,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C113" s="13">
         <v>111</v>
@@ -9887,7 +9901,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C114" s="13">
         <v>112</v>
@@ -9922,7 +9936,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C115" s="13">
         <v>113</v>
@@ -9957,7 +9971,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C116" s="24">
         <v>114</v>
@@ -9977,7 +9991,7 @@
         <v>STATION; GLENBURY</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I116" s="13">
         <f t="shared" si="10"/>
@@ -9998,7 +10012,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C117" s="13">
         <v>115</v>
@@ -10033,7 +10047,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C118" s="13">
         <v>116</v>
@@ -10068,7 +10082,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C119" s="13">
         <v>117</v>
@@ -10103,7 +10117,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C120" s="24">
         <v>118</v>
@@ -10138,7 +10152,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C121" s="13">
         <v>119</v>
@@ -10173,7 +10187,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C122" s="13">
         <v>120</v>
@@ -10208,7 +10222,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C123" s="13">
         <v>121</v>
@@ -10243,7 +10257,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C124" s="24">
         <v>122</v>
@@ -10280,7 +10294,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C125" s="13">
         <v>123</v>
@@ -10299,7 +10313,7 @@
         <v xml:space="preserve">UNDERGROUND; STATION; OVERBROOK; </v>
       </c>
       <c r="H125" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I125" s="13">
         <f t="shared" si="10"/>
@@ -10320,7 +10334,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C126" s="13">
         <v>124</v>
@@ -10357,7 +10371,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C127" s="13">
         <v>125</v>
@@ -10394,7 +10408,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C128" s="24">
         <v>126</v>
@@ -10431,7 +10445,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C129" s="13">
         <v>127</v>
@@ -10468,7 +10482,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C130" s="13">
         <v>128</v>
@@ -10505,7 +10519,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C131" s="13">
         <v>129</v>
@@ -10542,7 +10556,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C132" s="24">
         <v>130</v>
@@ -10579,7 +10593,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C133" s="13">
         <v>131</v>
@@ -10616,7 +10630,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C134" s="13">
         <v>132</v>
@@ -10635,7 +10649,7 @@
         <v xml:space="preserve">UNDERGROUND; STATION; INGLEWOOD; </v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I134" s="13">
         <f t="shared" si="10"/>
@@ -10656,7 +10670,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C135" s="13">
         <v>133</v>
@@ -10693,7 +10707,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C136" s="24">
         <v>134</v>
@@ -10730,7 +10744,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C137" s="13">
         <v>135</v>
@@ -10767,7 +10781,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C138" s="13">
         <v>136</v>
@@ -10804,7 +10818,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C139" s="13">
         <v>137</v>
@@ -10841,7 +10855,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C140" s="24">
         <v>138</v>
@@ -10878,7 +10892,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C141" s="13">
         <v>139</v>
@@ -10915,7 +10929,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C142" s="13">
         <v>140</v>
@@ -10952,7 +10966,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C143" s="13">
         <v>141</v>
@@ -10971,7 +10985,7 @@
         <v xml:space="preserve">UNDERGROUND; STATION; CENTRAL; </v>
       </c>
       <c r="H143" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I143" s="13">
         <f t="shared" si="10"/>
@@ -10992,7 +11006,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C144" s="24">
         <v>142</v>
@@ -11029,7 +11043,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C145" s="13">
         <v>143</v>
@@ -11066,7 +11080,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C146" s="13">
         <v>144</v>
@@ -11101,7 +11115,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C147" s="13">
         <v>145</v>
@@ -11136,7 +11150,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C148" s="24">
         <v>146</v>
@@ -11171,7 +11185,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C149" s="13">
         <v>147</v>
@@ -11206,7 +11220,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C150" s="13">
         <v>148</v>
@@ -11242,7 +11256,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C151" s="13">
         <v>149</v>
@@ -11277,7 +11291,7 @@
         <v>Green</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C152" s="24">
         <v>150</v>
@@ -11327,7 +11341,10 @@
       <c r="B155" s="13"/>
       <c r="C155" s="13"/>
       <c r="D155" s="13"/>
-      <c r="E155" s="13"/>
+      <c r="E155" s="13">
+        <f>SUM(D3:D152)</f>
+        <v>14552.6</v>
+      </c>
       <c r="F155" s="13"/>
       <c r="G155" s="13"/>
       <c r="H155" s="13"/>
@@ -11347,41 +11364,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="A2" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E8" s="8"/>
@@ -11434,6 +11451,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94389a86-b516-41d7-b262-f628eedfce35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="092657b9-1ee8-45be-93eb-ecd6d49d389e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087E6AE00E2F3594D99A2EDD8C640C429" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd43e735e3efd8f35f868d67510f3339">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="94389a86-b516-41d7-b262-f628eedfce35" xmlns:ns3="092657b9-1ee8-45be-93eb-ecd6d49d389e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0cc9a74db4250b9452c0be7dadb86fb" ns2:_="" ns3:_="">
     <xsd:import namespace="94389a86-b516-41d7-b262-f628eedfce35"/>
@@ -11644,41 +11681,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94389a86-b516-41d7-b262-f628eedfce35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="092657b9-1ee8-45be-93eb-ecd6d49d389e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90296A00-EB25-44C6-9222-0DA87540D231}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774DA102-3956-4D07-9A62-27A1AD8C69CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="94389a86-b516-41d7-b262-f628eedfce35"/>
-    <ds:schemaRef ds:uri="092657b9-1ee8-45be-93eb-ecd6d49d389e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11701,9 +11707,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774DA102-3956-4D07-9A62-27A1AD8C69CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90296A00-EB25-44C6-9222-0DA87540D231}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="94389a86-b516-41d7-b262-f628eedfce35"/>
+    <ds:schemaRef ds:uri="092657b9-1ee8-45be-93eb-ecd6d49d389e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
multiple trains merge fix
</commit_message>
<xml_diff>
--- a/Track Layout & Vehicle Data vF2.xlsx
+++ b/Track Layout & Vehicle Data vF2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshuttleworth/Desktop/ECE 1140/trains/ECE1140/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshuttleworth/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8460D32-93D5-2D4E-9872-542B2F7AAA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A932B1DD-D1F6-C845-AD8C-8CB8ED3D8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="32620" windowHeight="20500" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -170,25 +170,16 @@
     <t>UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; PENN STATION; UNDERGROUND</t>
-  </si>
-  <si>
     <t>SWITCH (27-28; 27-76); UNDERGROUND</t>
   </si>
   <si>
     <t>SWITCH (33-32; 33-72); UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION;     STEEL PLAZA; UNDERGROUND</t>
-  </si>
-  <si>
     <t>SWITCH (38-39; 38-71); UNDERGROUND</t>
   </si>
   <si>
     <t>SWITCH (44-43, 44-67); UNDERGROUND</t>
-  </si>
-  <si>
-    <t>STATION; FIRST AVE; UNDERGROUND</t>
   </si>
   <si>
     <t>I</t>
@@ -340,6 +331,15 @@
   <si>
     <t xml:space="preserve">UNDERGROUND; STATION; OVERBROOK; </t>
   </si>
+  <si>
+    <t>UNDERGROUND; STATION; PENN STATION</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; STATION; STEEL PLAZA</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; STATION; FIRST AVE</t>
+  </si>
 </sst>
 </file>
 
@@ -350,9 +350,16 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -467,30 +474,30 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -499,53 +506,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2256,9 +2269,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M45" sqref="M45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2311,7 +2324,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -2582,7 +2595,7 @@
       <c r="F9" s="13">
         <v>40</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="33" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="13" t="s">
@@ -2962,7 +2975,7 @@
       <c r="F19" s="13">
         <v>55</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="G19" s="33" t="s">
         <v>37</v>
       </c>
       <c r="H19" s="13" t="s">
@@ -3107,7 +3120,7 @@
       <c r="F23" s="13">
         <v>55</v>
       </c>
-      <c r="G23" s="19" t="s">
+      <c r="G23" s="33" t="s">
         <v>39</v>
       </c>
       <c r="H23" s="13" t="s">
@@ -3253,8 +3266,8 @@
       <c r="F27" s="13">
         <v>70</v>
       </c>
-      <c r="G27" s="19" t="s">
-        <v>42</v>
+      <c r="G27" s="33" t="s">
+        <v>96</v>
       </c>
       <c r="H27" s="13" t="s">
         <v>28</v>
@@ -3330,7 +3343,7 @@
         <v>70</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="25">
@@ -3552,7 +3565,7 @@
         <v>70</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="25">
@@ -3625,8 +3638,8 @@
       <c r="F37" s="13">
         <v>70</v>
       </c>
-      <c r="G37" s="19" t="s">
-        <v>45</v>
+      <c r="G37" s="33" t="s">
+        <v>97</v>
       </c>
       <c r="H37" s="13" t="s">
         <v>28</v>
@@ -3739,7 +3752,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="25">
@@ -3961,7 +3974,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="25">
@@ -3997,8 +4010,8 @@
       <c r="F47" s="13">
         <v>70</v>
       </c>
-      <c r="G47" s="19" t="s">
-        <v>48</v>
+      <c r="G47" s="33" t="s">
+        <v>98</v>
       </c>
       <c r="H47" s="13" t="s">
         <v>28</v>
@@ -4022,7 +4035,7 @@
         <v>Red</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C48" s="13">
         <v>46</v>
@@ -4059,7 +4072,7 @@
         <v>Red</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C49" s="24">
         <v>47</v>
@@ -4074,7 +4087,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="25">
@@ -4096,7 +4109,7 @@
         <v>Red</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C50" s="13">
         <v>48</v>
@@ -4111,7 +4124,7 @@
         <v>70</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H50" s="13" t="s">
         <v>28</v>
@@ -4135,7 +4148,7 @@
         <v>Red</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C51" s="13">
         <v>49</v>
@@ -4170,7 +4183,7 @@
         <v>Red</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C52" s="24">
         <v>50</v>
@@ -4205,7 +4218,7 @@
         <v>Red</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C53" s="13">
         <v>51</v>
@@ -4240,7 +4253,7 @@
         <v>Red</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C54" s="13">
         <v>52</v>
@@ -4255,7 +4268,7 @@
         <v>55</v>
       </c>
       <c r="G54" s="21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H54" s="13"/>
       <c r="I54" s="25">
@@ -4277,7 +4290,7 @@
         <v>Red</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C55" s="24">
         <v>53</v>
@@ -4312,7 +4325,7 @@
         <v>Red</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C56" s="13">
         <v>54</v>
@@ -4347,7 +4360,7 @@
         <v>Red</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C57" s="13">
         <v>55</v>
@@ -4382,7 +4395,7 @@
         <v>Red</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C58" s="24">
         <v>56</v>
@@ -4417,7 +4430,7 @@
         <v>Red</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C59" s="13">
         <v>57</v>
@@ -4452,7 +4465,7 @@
         <v>Red</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C60" s="13">
         <v>58</v>
@@ -4487,7 +4500,7 @@
         <v>Red</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C61" s="24">
         <v>59</v>
@@ -4522,7 +4535,7 @@
         <v>Red</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C62" s="13">
         <v>60</v>
@@ -4537,7 +4550,7 @@
         <v>55</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H62" s="13" t="s">
         <v>28</v>
@@ -4561,7 +4574,7 @@
         <v>Red</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C63" s="13">
         <v>61</v>
@@ -4596,7 +4609,7 @@
         <v>Red</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C64" s="24">
         <v>62</v>
@@ -4631,7 +4644,7 @@
         <v>Red</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C65" s="13">
         <v>63</v>
@@ -4666,7 +4679,7 @@
         <v>Red</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C66" s="13">
         <v>64</v>
@@ -4701,7 +4714,7 @@
         <v>Red</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C67" s="24">
         <v>65</v>
@@ -4736,7 +4749,7 @@
         <v>Red</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C68" s="13">
         <v>66</v>
@@ -4771,7 +4784,7 @@
         <v>Red</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C69" s="13">
         <v>67</v>
@@ -4808,7 +4821,7 @@
         <v>Red</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C70" s="24">
         <v>68</v>
@@ -4845,7 +4858,7 @@
         <v>Red</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C71" s="13">
         <v>69</v>
@@ -4882,7 +4895,7 @@
         <v>Red</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C72" s="13">
         <v>70</v>
@@ -4919,7 +4932,7 @@
         <v>Red</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C73" s="24">
         <v>71</v>
@@ -4956,7 +4969,7 @@
         <v>Red</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C74" s="13">
         <v>72</v>
@@ -4993,7 +5006,7 @@
         <v>Red</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C75" s="13">
         <v>73</v>
@@ -5030,7 +5043,7 @@
         <v>Red</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C76" s="24">
         <v>74</v>
@@ -5067,7 +5080,7 @@
         <v>Red</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C77" s="13">
         <v>75</v>
@@ -5104,7 +5117,7 @@
         <v>Red</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C78" s="13">
         <v>76</v>
@@ -5137,7 +5150,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="24"/>
@@ -5164,15 +5177,16 @@
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="B81" s="13"/>
       <c r="C81" s="24"/>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D81" s="34"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5180,7 +5194,7 @@
       <c r="B82" s="13"/>
       <c r="C82" s="24"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5188,7 +5202,7 @@
       <c r="B83" s="13"/>
       <c r="C83" s="24"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5196,7 +5210,7 @@
       <c r="B84" s="13"/>
       <c r="C84" s="24"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5204,7 +5218,7 @@
       <c r="B85" s="13"/>
       <c r="C85" s="24"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5212,7 +5226,7 @@
       <c r="B86" s="13"/>
       <c r="C86" s="24"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5220,7 +5234,7 @@
       <c r="B87" s="13"/>
       <c r="C87" s="24"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5228,7 +5242,7 @@
       <c r="B88" s="13"/>
       <c r="C88" s="24"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5236,7 +5250,7 @@
       <c r="B89" s="13"/>
       <c r="C89" s="24"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5244,7 +5258,7 @@
       <c r="B90" s="13"/>
       <c r="C90" s="24"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5252,7 +5266,7 @@
       <c r="B91" s="13"/>
       <c r="C91" s="24"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5260,7 +5274,7 @@
       <c r="B92" s="13"/>
       <c r="C92" s="24"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5268,7 +5282,7 @@
       <c r="B93" s="13"/>
       <c r="C93" s="24"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5276,7 +5290,7 @@
       <c r="B94" s="13"/>
       <c r="C94" s="24"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5284,7 +5298,7 @@
       <c r="B95" s="13"/>
       <c r="C95" s="24"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="13" t="str">
         <f t="shared" si="7"/>
         <v xml:space="preserve"> </v>
@@ -5774,9 +5788,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H58" sqref="H58"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G145" sqref="G145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5826,7 +5840,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -5843,7 +5857,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="6"/>
@@ -5854,7 +5868,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>13</v>
@@ -5909,10 +5923,10 @@
         <v>45</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I4" s="13">
         <f t="shared" ref="I4:I67" si="0">E4*D4/100</f>
@@ -6178,10 +6192,10 @@
         <v>45</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="0"/>
@@ -6334,7 +6348,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13">
@@ -6445,7 +6459,7 @@
         <v>70</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H18" s="13" t="s">
         <v>28</v>
@@ -6554,7 +6568,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13">
@@ -6661,7 +6675,7 @@
         <v>70</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H24" s="13" t="s">
         <v>28</v>
@@ -6875,7 +6889,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13">
@@ -6982,10 +6996,10 @@
         <v>30</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I33" s="13">
         <f t="shared" si="0"/>
@@ -7146,7 +7160,7 @@
         <v>Green</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C38" s="13">
         <v>36</v>
@@ -7183,7 +7197,7 @@
         <v>Green</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C39" s="13">
         <v>37</v>
@@ -7220,7 +7234,7 @@
         <v>Green</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C40" s="24">
         <v>38</v>
@@ -7257,7 +7271,7 @@
         <v>Green</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C41" s="13">
         <v>39</v>
@@ -7271,11 +7285,11 @@
       <c r="F41" s="13">
         <v>30</v>
       </c>
-      <c r="G41" s="32" t="s">
-        <v>96</v>
+      <c r="G41" s="30" t="s">
+        <v>93</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I41" s="13">
         <f t="shared" si="0"/>
@@ -7296,7 +7310,7 @@
         <v>Green</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C42" s="13">
         <v>40</v>
@@ -7333,7 +7347,7 @@
         <v>Green</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C43" s="24">
         <v>41</v>
@@ -7370,7 +7384,7 @@
         <v>Green</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C44" s="13">
         <v>42</v>
@@ -7407,7 +7421,7 @@
         <v>Green</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C45" s="13">
         <v>43</v>
@@ -7444,7 +7458,7 @@
         <v>Green</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C46" s="24">
         <v>44</v>
@@ -7481,7 +7495,7 @@
         <v>Green</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C47" s="13">
         <v>45</v>
@@ -7518,7 +7532,7 @@
         <v>Green</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C48" s="13">
         <v>46</v>
@@ -7555,7 +7569,7 @@
         <v>Green</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C49" s="24">
         <v>47</v>
@@ -7592,7 +7606,7 @@
         <v>Green</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C50" s="13">
         <v>48</v>
@@ -7606,11 +7620,11 @@
       <c r="F50" s="13">
         <v>30</v>
       </c>
-      <c r="G50" s="32" t="s">
-        <v>97</v>
+      <c r="G50" s="30" t="s">
+        <v>94</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I50" s="13">
         <f t="shared" si="0"/>
@@ -7631,7 +7645,7 @@
         <v>Green</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C51" s="13">
         <v>49</v>
@@ -7668,7 +7682,7 @@
         <v>Green</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C52" s="24">
         <v>50</v>
@@ -7705,7 +7719,7 @@
         <v>Green</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C53" s="13">
         <v>51</v>
@@ -7742,7 +7756,7 @@
         <v>Green</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C54" s="13">
         <v>52</v>
@@ -7779,7 +7793,7 @@
         <v>Green</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C55" s="24">
         <v>53</v>
@@ -7816,7 +7830,7 @@
         <v>Green</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C56" s="13">
         <v>54</v>
@@ -7853,7 +7867,7 @@
         <v>Green</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C57" s="13">
         <v>55</v>
@@ -7890,7 +7904,7 @@
         <v>Green</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C58" s="24">
         <v>56</v>
@@ -7904,8 +7918,8 @@
       <c r="F58" s="13">
         <v>30</v>
       </c>
-      <c r="G58" s="32" t="s">
-        <v>98</v>
+      <c r="G58" s="30" t="s">
+        <v>95</v>
       </c>
       <c r="H58" s="13"/>
       <c r="I58" s="13">
@@ -7927,7 +7941,7 @@
         <v>Green</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C59" s="13">
         <v>57</v>
@@ -7942,10 +7956,10 @@
         <v>30</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I59" s="13">
         <f t="shared" si="0"/>
@@ -7966,7 +7980,7 @@
         <v>Green</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C60" s="13">
         <v>58</v>
@@ -8001,7 +8015,7 @@
         <v>Green</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C61" s="24">
         <v>59</v>
@@ -8036,7 +8050,7 @@
         <v>Green</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C62" s="13">
         <v>60</v>
@@ -8071,7 +8085,7 @@
         <v>Green</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C63" s="13">
         <v>61</v>
@@ -8106,7 +8120,7 @@
         <v>Green</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C64" s="24">
         <v>62</v>
@@ -8141,7 +8155,7 @@
         <v>Green</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C65" s="13">
         <v>63</v>
@@ -8156,7 +8170,7 @@
         <v>70</v>
       </c>
       <c r="G65" s="21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H65" s="13"/>
       <c r="I65" s="13">
@@ -8178,7 +8192,7 @@
         <v>Green</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C66" s="13">
         <v>64</v>
@@ -8213,7 +8227,7 @@
         <v>Green</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C67" s="24">
         <v>65</v>
@@ -8228,10 +8242,10 @@
         <v>70</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I67" s="13">
         <f t="shared" si="0"/>
@@ -8252,7 +8266,7 @@
         <v>Green</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C68" s="13">
         <v>66</v>
@@ -8287,7 +8301,7 @@
         <v>Green</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C69" s="13">
         <v>67</v>
@@ -8322,7 +8336,7 @@
         <v>Green</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C70" s="24">
         <v>68</v>
@@ -8357,7 +8371,7 @@
         <v>Green</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C71" s="13">
         <v>69</v>
@@ -8392,7 +8406,7 @@
         <v>Green</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C72" s="13">
         <v>70</v>
@@ -8427,7 +8441,7 @@
         <v>Green</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C73" s="24">
         <v>71</v>
@@ -8462,7 +8476,7 @@
         <v>Green</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C74" s="13">
         <v>72</v>
@@ -8497,7 +8511,7 @@
         <v>Green</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C75" s="13">
         <v>73</v>
@@ -8512,10 +8526,10 @@
         <v>40</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I75" s="13">
         <f t="shared" si="5"/>
@@ -8536,7 +8550,7 @@
         <v>Green</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C76" s="24">
         <v>74</v>
@@ -8571,7 +8585,7 @@
         <v>Green</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C77" s="13">
         <v>75</v>
@@ -8606,7 +8620,7 @@
         <v>Green</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C78" s="13">
         <v>76</v>
@@ -8641,7 +8655,7 @@
         <v>Green</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C79" s="13">
         <v>77</v>
@@ -8656,7 +8670,7 @@
         <v>70</v>
       </c>
       <c r="G79" s="21" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="H79" s="13"/>
       <c r="I79" s="13">
@@ -8678,7 +8692,7 @@
         <v>Green</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C80" s="24">
         <v>78</v>
@@ -8693,7 +8707,7 @@
         <v>70</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="H80" s="13" t="s">
         <v>28</v>
@@ -8717,7 +8731,7 @@
         <v>Green</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C81" s="13">
         <v>79</v>
@@ -8752,7 +8766,7 @@
         <v>Green</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C82" s="13">
         <v>80</v>
@@ -8787,7 +8801,7 @@
         <v>Green</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C83" s="13">
         <v>81</v>
@@ -8822,7 +8836,7 @@
         <v>Green</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C84" s="24">
         <v>82</v>
@@ -8857,7 +8871,7 @@
         <v>Green</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C85" s="13">
         <v>83</v>
@@ -8892,7 +8906,7 @@
         <v>Green</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C86" s="13">
         <v>84</v>
@@ -8927,7 +8941,7 @@
         <v>Green</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C87" s="13">
         <v>85</v>
@@ -8942,7 +8956,7 @@
         <v>70</v>
       </c>
       <c r="G87" s="21" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="13">
@@ -8964,7 +8978,7 @@
         <v>Green</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C88" s="24">
         <v>86</v>
@@ -8999,7 +9013,7 @@
         <v>Green</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C89" s="13">
         <v>87</v>
@@ -9034,7 +9048,7 @@
         <v>Green</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C90" s="13">
         <v>88</v>
@@ -9049,10 +9063,10 @@
         <v>25</v>
       </c>
       <c r="G90" s="19" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I90" s="13">
         <f t="shared" si="8"/>
@@ -9073,7 +9087,7 @@
         <v>Green</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C91" s="13">
         <v>89</v>
@@ -9108,7 +9122,7 @@
         <v>Green</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C92" s="24">
         <v>90</v>
@@ -9143,7 +9157,7 @@
         <v>Green</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C93" s="13">
         <v>91</v>
@@ -9178,7 +9192,7 @@
         <v>Green</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C94" s="13">
         <v>92</v>
@@ -9213,7 +9227,7 @@
         <v>Green</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C95" s="13">
         <v>93</v>
@@ -9248,7 +9262,7 @@
         <v>Green</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C96" s="24">
         <v>94</v>
@@ -9283,7 +9297,7 @@
         <v>Green</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C97" s="13">
         <v>95</v>
@@ -9318,7 +9332,7 @@
         <v>Green</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C98" s="13">
         <v>96</v>
@@ -9333,10 +9347,10 @@
         <v>25</v>
       </c>
       <c r="G98" s="19" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I98" s="13">
         <f t="shared" si="8"/>
@@ -9357,7 +9371,7 @@
         <v>Green</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C99" s="13">
         <v>97</v>
@@ -9392,7 +9406,7 @@
         <v>Green</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C100" s="24">
         <v>98</v>
@@ -9427,7 +9441,7 @@
         <v>Green</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C101" s="13">
         <v>99</v>
@@ -9462,7 +9476,7 @@
         <v>Green</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C102" s="13">
         <v>100</v>
@@ -9497,7 +9511,7 @@
         <v>Green</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C103" s="13">
         <v>101</v>
@@ -9532,7 +9546,7 @@
         <v>Green</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C104" s="24">
         <v>102</v>
@@ -9567,7 +9581,7 @@
         <v>Green</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C105" s="13">
         <v>103</v>
@@ -9602,7 +9616,7 @@
         <v>Green</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C106" s="13">
         <v>104</v>
@@ -9637,7 +9651,7 @@
         <v>Green</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C107" s="13">
         <v>105</v>
@@ -9656,7 +9670,7 @@
         <v>STATION; DORMONT</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I107" s="13">
         <f t="shared" si="8"/>
@@ -9677,7 +9691,7 @@
         <v>Green</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C108" s="24">
         <v>106</v>
@@ -9712,7 +9726,7 @@
         <v>Green</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C109" s="13">
         <v>107</v>
@@ -9747,7 +9761,7 @@
         <v>Green</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C110" s="13">
         <v>108</v>
@@ -9782,7 +9796,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C111" s="13">
         <v>109</v>
@@ -9817,7 +9831,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C112" s="24">
         <v>110</v>
@@ -9852,7 +9866,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C113" s="13">
         <v>111</v>
@@ -9887,7 +9901,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C114" s="13">
         <v>112</v>
@@ -9922,7 +9936,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C115" s="13">
         <v>113</v>
@@ -9957,7 +9971,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C116" s="24">
         <v>114</v>
@@ -9977,7 +9991,7 @@
         <v>STATION; GLENBURY</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I116" s="13">
         <f t="shared" si="10"/>
@@ -9998,7 +10012,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C117" s="13">
         <v>115</v>
@@ -10033,7 +10047,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C118" s="13">
         <v>116</v>
@@ -10068,7 +10082,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C119" s="13">
         <v>117</v>
@@ -10103,7 +10117,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C120" s="24">
         <v>118</v>
@@ -10138,7 +10152,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C121" s="13">
         <v>119</v>
@@ -10173,7 +10187,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C122" s="13">
         <v>120</v>
@@ -10208,7 +10222,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C123" s="13">
         <v>121</v>
@@ -10243,7 +10257,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C124" s="24">
         <v>122</v>
@@ -10280,7 +10294,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C125" s="13">
         <v>123</v>
@@ -10299,7 +10313,7 @@
         <v xml:space="preserve">UNDERGROUND; STATION; OVERBROOK; </v>
       </c>
       <c r="H125" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I125" s="13">
         <f t="shared" si="10"/>
@@ -10320,7 +10334,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C126" s="13">
         <v>124</v>
@@ -10357,7 +10371,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C127" s="13">
         <v>125</v>
@@ -10394,7 +10408,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C128" s="24">
         <v>126</v>
@@ -10431,7 +10445,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C129" s="13">
         <v>127</v>
@@ -10468,7 +10482,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C130" s="13">
         <v>128</v>
@@ -10505,7 +10519,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C131" s="13">
         <v>129</v>
@@ -10542,7 +10556,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C132" s="24">
         <v>130</v>
@@ -10579,7 +10593,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C133" s="13">
         <v>131</v>
@@ -10616,7 +10630,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C134" s="13">
         <v>132</v>
@@ -10635,7 +10649,7 @@
         <v xml:space="preserve">UNDERGROUND; STATION; INGLEWOOD; </v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="I134" s="13">
         <f t="shared" si="10"/>
@@ -10656,7 +10670,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C135" s="13">
         <v>133</v>
@@ -10693,7 +10707,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C136" s="24">
         <v>134</v>
@@ -10730,7 +10744,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C137" s="13">
         <v>135</v>
@@ -10767,7 +10781,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C138" s="13">
         <v>136</v>
@@ -10804,7 +10818,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C139" s="13">
         <v>137</v>
@@ -10841,7 +10855,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C140" s="24">
         <v>138</v>
@@ -10878,7 +10892,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C141" s="13">
         <v>139</v>
@@ -10915,7 +10929,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C142" s="13">
         <v>140</v>
@@ -10952,7 +10966,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C143" s="13">
         <v>141</v>
@@ -10971,7 +10985,7 @@
         <v xml:space="preserve">UNDERGROUND; STATION; CENTRAL; </v>
       </c>
       <c r="H143" s="13" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I143" s="13">
         <f t="shared" si="10"/>
@@ -10992,7 +11006,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C144" s="24">
         <v>142</v>
@@ -11029,7 +11043,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C145" s="13">
         <v>143</v>
@@ -11066,7 +11080,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C146" s="13">
         <v>144</v>
@@ -11101,7 +11115,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C147" s="13">
         <v>145</v>
@@ -11136,7 +11150,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C148" s="24">
         <v>146</v>
@@ -11171,7 +11185,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C149" s="13">
         <v>147</v>
@@ -11206,7 +11220,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C150" s="13">
         <v>148</v>
@@ -11242,7 +11256,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C151" s="13">
         <v>149</v>
@@ -11277,7 +11291,7 @@
         <v>Green</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C152" s="24">
         <v>150</v>
@@ -11327,7 +11341,10 @@
       <c r="B155" s="13"/>
       <c r="C155" s="13"/>
       <c r="D155" s="13"/>
-      <c r="E155" s="13"/>
+      <c r="E155" s="13">
+        <f>SUM(D3:D152)</f>
+        <v>14552.6</v>
+      </c>
       <c r="F155" s="13"/>
       <c r="G155" s="13"/>
       <c r="H155" s="13"/>
@@ -11354,34 +11371,34 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
+      <c r="A1" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="30"/>
+      <c r="A2" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E8" s="8"/>
@@ -11434,6 +11451,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94389a86-b516-41d7-b262-f628eedfce35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="092657b9-1ee8-45be-93eb-ecd6d49d389e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087E6AE00E2F3594D99A2EDD8C640C429" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd43e735e3efd8f35f868d67510f3339">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="94389a86-b516-41d7-b262-f628eedfce35" xmlns:ns3="092657b9-1ee8-45be-93eb-ecd6d49d389e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0cc9a74db4250b9452c0be7dadb86fb" ns2:_="" ns3:_="">
     <xsd:import namespace="94389a86-b516-41d7-b262-f628eedfce35"/>
@@ -11644,41 +11681,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94389a86-b516-41d7-b262-f628eedfce35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="092657b9-1ee8-45be-93eb-ecd6d49d389e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90296A00-EB25-44C6-9222-0DA87540D231}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774DA102-3956-4D07-9A62-27A1AD8C69CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="94389a86-b516-41d7-b262-f628eedfce35"/>
-    <ds:schemaRef ds:uri="092657b9-1ee8-45be-93eb-ecd6d49d389e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11701,9 +11707,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774DA102-3956-4D07-9A62-27A1AD8C69CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90296A00-EB25-44C6-9222-0DA87540D231}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="94389a86-b516-41d7-b262-f628eedfce35"/>
+    <ds:schemaRef ds:uri="092657b9-1ee8-45be-93eb-ecd6d49d389e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes implemented, bug fixes needed
</commit_message>
<xml_diff>
--- a/Track Layout & Vehicle Data vF2.xlsx
+++ b/Track Layout & Vehicle Data vF2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshuttleworth/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshuttleworth/Desktop/ECE 1140/trains/ECE1140/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A932B1DD-D1F6-C845-AD8C-8CB8ED3D8ED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3646A123-DB9A-184D-8CA2-1014AE49E1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="920" yWindow="500" windowWidth="19200" windowHeight="20500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -548,17 +548,17 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2270,8 +2270,8 @@
   <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2337,7 +2337,9 @@
       <c r="C2" s="24">
         <v>0</v>
       </c>
-      <c r="D2" s="13"/>
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
       <c r="G2" s="22" t="s">
@@ -2595,7 +2597,7 @@
       <c r="F9" s="13">
         <v>40</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="31" t="s">
         <v>27</v>
       </c>
       <c r="H9" s="13" t="s">
@@ -2975,7 +2977,7 @@
       <c r="F19" s="13">
         <v>55</v>
       </c>
-      <c r="G19" s="33" t="s">
+      <c r="G19" s="31" t="s">
         <v>37</v>
       </c>
       <c r="H19" s="13" t="s">
@@ -3120,7 +3122,7 @@
       <c r="F23" s="13">
         <v>55</v>
       </c>
-      <c r="G23" s="33" t="s">
+      <c r="G23" s="31" t="s">
         <v>39</v>
       </c>
       <c r="H23" s="13" t="s">
@@ -3266,7 +3268,7 @@
       <c r="F27" s="13">
         <v>70</v>
       </c>
-      <c r="G27" s="33" t="s">
+      <c r="G27" s="31" t="s">
         <v>96</v>
       </c>
       <c r="H27" s="13" t="s">
@@ -3638,7 +3640,7 @@
       <c r="F37" s="13">
         <v>70</v>
       </c>
-      <c r="G37" s="33" t="s">
+      <c r="G37" s="31" t="s">
         <v>97</v>
       </c>
       <c r="H37" s="13" t="s">
@@ -4010,7 +4012,7 @@
       <c r="F47" s="13">
         <v>70</v>
       </c>
-      <c r="G47" s="33" t="s">
+      <c r="G47" s="31" t="s">
         <v>98</v>
       </c>
       <c r="H47" s="13" t="s">
@@ -5184,7 +5186,7 @@
       </c>
       <c r="B81" s="13"/>
       <c r="C81" s="24"/>
-      <c r="D81" s="34"/>
+      <c r="D81" s="32"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="str">
@@ -5789,8 +5791,8 @@
   <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G145" sqref="G145"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5853,7 +5855,9 @@
       <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="13" t="s">
@@ -11371,34 +11375,34 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E8" s="8"/>
@@ -11451,26 +11455,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94389a86-b516-41d7-b262-f628eedfce35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="092657b9-1ee8-45be-93eb-ecd6d49d389e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010087E6AE00E2F3594D99A2EDD8C640C429" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dd43e735e3efd8f35f868d67510f3339">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="94389a86-b516-41d7-b262-f628eedfce35" xmlns:ns3="092657b9-1ee8-45be-93eb-ecd6d49d389e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b0cc9a74db4250b9452c0be7dadb86fb" ns2:_="" ns3:_="">
     <xsd:import namespace="94389a86-b516-41d7-b262-f628eedfce35"/>
@@ -11681,10 +11665,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="94389a86-b516-41d7-b262-f628eedfce35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="092657b9-1ee8-45be-93eb-ecd6d49d389e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774DA102-3956-4D07-9A62-27A1AD8C69CE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90296A00-EB25-44C6-9222-0DA87540D231}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="94389a86-b516-41d7-b262-f628eedfce35"/>
+    <ds:schemaRef ds:uri="092657b9-1ee8-45be-93eb-ecd6d49d389e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -11707,20 +11722,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90296A00-EB25-44C6-9222-0DA87540D231}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{774DA102-3956-4D07-9A62-27A1AD8C69CE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="94389a86-b516-41d7-b262-f628eedfce35"/>
-    <ds:schemaRef ds:uri="092657b9-1ee8-45be-93eb-ecd6d49d389e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed error in excel sheet
</commit_message>
<xml_diff>
--- a/Track Layout & Vehicle Data vF2.xlsx
+++ b/Track Layout & Vehicle Data vF2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshuttleworth/Desktop/ECE 1140/trains/ECE1140/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3646A123-DB9A-184D-8CA2-1014AE49E1D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181DFBED-2460-274E-B782-C18E77961222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="920" yWindow="500" windowWidth="19200" windowHeight="20500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="99">
   <si>
     <t>Release 2.0 of Track data - corrections shown in yellow cells; see red and green line</t>
   </si>
@@ -350,9 +350,16 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -474,30 +481,30 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -506,59 +513,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2269,9 +2279,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5790,9 +5800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L58" sqref="L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7925,7 +7935,9 @@
       <c r="G58" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="H58" s="13"/>
+      <c r="H58" s="35" t="s">
+        <v>74</v>
+      </c>
       <c r="I58" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -9023,7 +9035,7 @@
         <v>87</v>
       </c>
       <c r="D89" s="13">
-        <v>86.6</v>
+        <v>90</v>
       </c>
       <c r="E89" s="13">
         <v>0</v>
@@ -9043,7 +9055,7 @@
       </c>
       <c r="K89" s="28">
         <f t="shared" si="4"/>
-        <v>12.470399999999998</v>
+        <v>12.959999999999999</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -11347,7 +11359,7 @@
       <c r="D155" s="13"/>
       <c r="E155" s="13">
         <f>SUM(D3:D152)</f>
-        <v>14552.6</v>
+        <v>14556</v>
       </c>
       <c r="F155" s="13"/>
       <c r="G155" s="13"/>
@@ -11361,6 +11373,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed excel sheet again
</commit_message>
<xml_diff>
--- a/Track Layout & Vehicle Data vF2.xlsx
+++ b/Track Layout & Vehicle Data vF2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benshuttleworth/Desktop/ECE 1140/trains/ECE1140/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181DFBED-2460-274E-B782-C18E77961222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51A3A0A8-40B0-0747-B39C-DB92D93D99C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="3" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>Junction Switch</t>
   </si>
   <si>
-    <t>STATION: SHADYSIDE</t>
-  </si>
-  <si>
     <t>Left/Right</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
   </si>
   <si>
     <t>SWITCH (16-1, 16-15)</t>
-  </si>
-  <si>
-    <t>STATION: HERRON AVE</t>
   </si>
   <si>
     <t>G</t>
@@ -293,9 +287,6 @@
     <t>STATION; POPLAR</t>
   </si>
   <si>
-    <t>STATION;   CASTLE SHANNON</t>
-  </si>
-  <si>
     <t>U</t>
   </si>
   <si>
@@ -323,15 +314,6 @@
     <t>The lowest block number is closest to the letter in the alphabet preceding the block section letter.</t>
   </si>
   <si>
-    <t xml:space="preserve">UNDERGROUND; STATION; CENTRAL; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNDERGROUND; STATION; INGLEWOOD; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNDERGROUND; STATION; OVERBROOK; </t>
-  </si>
-  <si>
     <t>UNDERGROUND; STATION; PENN STATION</t>
   </si>
   <si>
@@ -339,6 +321,24 @@
   </si>
   <si>
     <t>UNDERGROUND; STATION; FIRST AVE</t>
+  </si>
+  <si>
+    <t>STATION; CASTLE SHANNON</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; STATION; CENTRAL</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; STATION; INGLEWOOD</t>
+  </si>
+  <si>
+    <t>UNDERGROUND; STATION; OVERBROOK</t>
+  </si>
+  <si>
+    <t>STATION; SHADYSIDE</t>
+  </si>
+  <si>
+    <t>STATION; HERRON AVE</t>
   </si>
 </sst>
 </file>
@@ -350,16 +350,9 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -481,30 +474,30 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -513,46 +506,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -561,14 +551,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2279,9 +2272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D78"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2334,7 +2327,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -2607,11 +2600,11 @@
       <c r="F9" s="13">
         <v>40</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>27</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>28</v>
       </c>
       <c r="I9" s="25">
         <f t="shared" si="0"/>
@@ -2627,7 +2620,7 @@
       </c>
       <c r="L9" s="14"/>
       <c r="M9" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -2666,7 +2659,7 @@
       </c>
       <c r="L10" s="14"/>
       <c r="M10" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -2690,7 +2683,7 @@
         <v>40</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="13"/>
       <c r="I11" s="25">
@@ -2707,7 +2700,7 @@
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -2716,7 +2709,7 @@
         <v>Red</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="24">
         <v>10</v>
@@ -2753,7 +2746,7 @@
         <v>Red</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" s="13">
         <v>11</v>
@@ -2790,7 +2783,7 @@
         <v>Red</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="24">
         <v>12</v>
@@ -2827,7 +2820,7 @@
         <v>Red</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="13">
         <v>13</v>
@@ -2864,7 +2857,7 @@
         <v>Red</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="13">
         <v>14</v>
@@ -2901,7 +2894,7 @@
         <v>Red</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="24">
         <v>15</v>
@@ -2936,7 +2929,7 @@
         <v>Red</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="13">
         <v>16</v>
@@ -2951,7 +2944,7 @@
         <v>40</v>
       </c>
       <c r="G18" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H18" s="13"/>
       <c r="I18" s="25">
@@ -2973,7 +2966,7 @@
         <v>Red</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="24">
         <v>17</v>
@@ -2987,11 +2980,11 @@
       <c r="F19" s="13">
         <v>55</v>
       </c>
-      <c r="G19" s="31" t="s">
-        <v>37</v>
+      <c r="G19" s="35" t="s">
+        <v>98</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I19" s="25">
         <f>E19*D19/100</f>
@@ -3012,7 +3005,7 @@
         <v>Red</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="13">
         <v>18</v>
@@ -3048,7 +3041,7 @@
         <v>Red</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C21" s="13">
         <v>19</v>
@@ -3083,7 +3076,7 @@
         <v>Red</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C22" s="24">
         <v>20</v>
@@ -3118,7 +3111,7 @@
         <v>Red</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="13">
         <v>21</v>
@@ -3132,11 +3125,11 @@
       <c r="F23" s="13">
         <v>55</v>
       </c>
-      <c r="G23" s="31" t="s">
-        <v>39</v>
+      <c r="G23" s="30" t="s">
+        <v>37</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I23" s="25">
         <f t="shared" si="0"/>
@@ -3157,7 +3150,7 @@
         <v>Red</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="24">
         <v>22</v>
@@ -3192,7 +3185,7 @@
         <v>Red</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C25" s="13">
         <v>23</v>
@@ -3227,7 +3220,7 @@
         <v>Red</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C26" s="13">
         <v>24</v>
@@ -3242,7 +3235,7 @@
         <v>70</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H26" s="13"/>
       <c r="I26" s="25">
@@ -3264,7 +3257,7 @@
         <v>Red</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C27" s="24">
         <v>25</v>
@@ -3278,11 +3271,11 @@
       <c r="F27" s="13">
         <v>70</v>
       </c>
-      <c r="G27" s="31" t="s">
-        <v>96</v>
+      <c r="G27" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I27" s="25">
         <f t="shared" si="0"/>
@@ -3303,7 +3296,7 @@
         <v>Red</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C28" s="13">
         <v>26</v>
@@ -3318,7 +3311,7 @@
         <v>70</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H28" s="13"/>
       <c r="I28" s="25">
@@ -3340,7 +3333,7 @@
         <v>Red</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="24">
         <v>27</v>
@@ -3355,7 +3348,7 @@
         <v>70</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H29" s="13"/>
       <c r="I29" s="25">
@@ -3377,7 +3370,7 @@
         <v>Red</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C30" s="13">
         <v>28</v>
@@ -3392,7 +3385,7 @@
         <v>70</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="25">
@@ -3414,7 +3407,7 @@
         <v>Red</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C31" s="13">
         <v>29</v>
@@ -3429,7 +3422,7 @@
         <v>70</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H31" s="13"/>
       <c r="I31" s="25">
@@ -3451,7 +3444,7 @@
         <v>Red</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" s="24">
         <v>30</v>
@@ -3466,7 +3459,7 @@
         <v>70</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H32" s="13"/>
       <c r="I32" s="25">
@@ -3488,7 +3481,7 @@
         <v>Red</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C33" s="13">
         <v>31</v>
@@ -3503,7 +3496,7 @@
         <v>70</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H33" s="13"/>
       <c r="I33" s="25">
@@ -3525,7 +3518,7 @@
         <v>Red</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C34" s="24">
         <v>32</v>
@@ -3540,7 +3533,7 @@
         <v>70</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H34" s="13"/>
       <c r="I34" s="25">
@@ -3562,7 +3555,7 @@
         <v>Red</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="13">
         <v>33</v>
@@ -3577,7 +3570,7 @@
         <v>70</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H35" s="13"/>
       <c r="I35" s="25">
@@ -3599,7 +3592,7 @@
         <v>Red</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="13">
         <v>34</v>
@@ -3614,7 +3607,7 @@
         <v>70</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H36" s="13"/>
       <c r="I36" s="25">
@@ -3636,7 +3629,7 @@
         <v>Red</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="24">
         <v>35</v>
@@ -3650,11 +3643,11 @@
       <c r="F37" s="13">
         <v>70</v>
       </c>
-      <c r="G37" s="31" t="s">
-        <v>97</v>
+      <c r="G37" s="30" t="s">
+        <v>91</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I37" s="25">
         <f t="shared" si="0"/>
@@ -3675,7 +3668,7 @@
         <v>Red</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" s="13">
         <v>36</v>
@@ -3690,7 +3683,7 @@
         <v>70</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="25">
@@ -3712,7 +3705,7 @@
         <v>Red</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C39" s="13">
         <v>37</v>
@@ -3727,7 +3720,7 @@
         <v>70</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="25">
@@ -3749,7 +3742,7 @@
         <v>Red</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C40" s="24">
         <v>38</v>
@@ -3764,7 +3757,7 @@
         <v>70</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="25">
@@ -3786,7 +3779,7 @@
         <v>Red</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C41" s="13">
         <v>39</v>
@@ -3801,7 +3794,7 @@
         <v>70</v>
       </c>
       <c r="G41" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H41" s="13"/>
       <c r="I41" s="25">
@@ -3823,7 +3816,7 @@
         <v>Red</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C42" s="13">
         <v>40</v>
@@ -3838,7 +3831,7 @@
         <v>70</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="25">
@@ -3860,7 +3853,7 @@
         <v>Red</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C43" s="24">
         <v>41</v>
@@ -3875,7 +3868,7 @@
         <v>70</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="25">
@@ -3897,7 +3890,7 @@
         <v>Red</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C44" s="13">
         <v>42</v>
@@ -3912,7 +3905,7 @@
         <v>70</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="25">
@@ -3934,7 +3927,7 @@
         <v>Red</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C45" s="13">
         <v>43</v>
@@ -3949,7 +3942,7 @@
         <v>70</v>
       </c>
       <c r="G45" s="23" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="25">
@@ -3971,7 +3964,7 @@
         <v>Red</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" s="24">
         <v>44</v>
@@ -3986,7 +3979,7 @@
         <v>70</v>
       </c>
       <c r="G46" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="25">
@@ -4008,7 +4001,7 @@
         <v>Red</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C47" s="13">
         <v>45</v>
@@ -4022,11 +4015,11 @@
       <c r="F47" s="13">
         <v>70</v>
       </c>
-      <c r="G47" s="31" t="s">
-        <v>98</v>
+      <c r="G47" s="30" t="s">
+        <v>92</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I47" s="25">
         <f t="shared" si="0"/>
@@ -4047,7 +4040,7 @@
         <v>Red</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C48" s="13">
         <v>46</v>
@@ -4062,7 +4055,7 @@
         <v>70</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="25">
@@ -4084,7 +4077,7 @@
         <v>Red</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C49" s="24">
         <v>47</v>
@@ -4099,7 +4092,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="25">
@@ -4121,7 +4114,7 @@
         <v>Red</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C50" s="13">
         <v>48</v>
@@ -4136,10 +4129,10 @@
         <v>70</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I50" s="25">
         <f t="shared" si="0"/>
@@ -4160,7 +4153,7 @@
         <v>Red</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C51" s="13">
         <v>49</v>
@@ -4195,7 +4188,7 @@
         <v>Red</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C52" s="24">
         <v>50</v>
@@ -4230,7 +4223,7 @@
         <v>Red</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C53" s="13">
         <v>51</v>
@@ -4265,7 +4258,7 @@
         <v>Red</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C54" s="13">
         <v>52</v>
@@ -4280,7 +4273,7 @@
         <v>55</v>
       </c>
       <c r="G54" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H54" s="13"/>
       <c r="I54" s="25">
@@ -4302,7 +4295,7 @@
         <v>Red</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C55" s="24">
         <v>53</v>
@@ -4337,7 +4330,7 @@
         <v>Red</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C56" s="13">
         <v>54</v>
@@ -4372,7 +4365,7 @@
         <v>Red</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C57" s="13">
         <v>55</v>
@@ -4407,7 +4400,7 @@
         <v>Red</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C58" s="24">
         <v>56</v>
@@ -4442,7 +4435,7 @@
         <v>Red</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C59" s="13">
         <v>57</v>
@@ -4477,7 +4470,7 @@
         <v>Red</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C60" s="13">
         <v>58</v>
@@ -4512,7 +4505,7 @@
         <v>Red</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C61" s="24">
         <v>59</v>
@@ -4547,7 +4540,7 @@
         <v>Red</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C62" s="13">
         <v>60</v>
@@ -4562,10 +4555,10 @@
         <v>55</v>
       </c>
       <c r="G62" s="19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I62" s="25">
         <f t="shared" si="0"/>
@@ -4586,7 +4579,7 @@
         <v>Red</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C63" s="13">
         <v>61</v>
@@ -4621,7 +4614,7 @@
         <v>Red</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C64" s="24">
         <v>62</v>
@@ -4656,7 +4649,7 @@
         <v>Red</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C65" s="13">
         <v>63</v>
@@ -4691,7 +4684,7 @@
         <v>Red</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C66" s="13">
         <v>64</v>
@@ -4726,7 +4719,7 @@
         <v>Red</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C67" s="24">
         <v>65</v>
@@ -4761,7 +4754,7 @@
         <v>Red</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C68" s="13">
         <v>66</v>
@@ -4796,7 +4789,7 @@
         <v>Red</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C69" s="13">
         <v>67</v>
@@ -4811,7 +4804,7 @@
         <v>55</v>
       </c>
       <c r="G69" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H69" s="13"/>
       <c r="I69" s="25">
@@ -4833,7 +4826,7 @@
         <v>Red</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C70" s="24">
         <v>68</v>
@@ -4848,7 +4841,7 @@
         <v>55</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H70" s="13"/>
       <c r="I70" s="25">
@@ -4870,7 +4863,7 @@
         <v>Red</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C71" s="13">
         <v>69</v>
@@ -4885,7 +4878,7 @@
         <v>55</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H71" s="13"/>
       <c r="I71" s="25">
@@ -4907,7 +4900,7 @@
         <v>Red</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C72" s="13">
         <v>70</v>
@@ -4922,7 +4915,7 @@
         <v>55</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H72" s="13"/>
       <c r="I72" s="25">
@@ -4944,7 +4937,7 @@
         <v>Red</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C73" s="24">
         <v>71</v>
@@ -4959,7 +4952,7 @@
         <v>55</v>
       </c>
       <c r="G73" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H73" s="13"/>
       <c r="I73" s="25">
@@ -4981,7 +4974,7 @@
         <v>Red</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C74" s="13">
         <v>72</v>
@@ -4996,7 +4989,7 @@
         <v>55</v>
       </c>
       <c r="G74" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H74" s="13"/>
       <c r="I74" s="25">
@@ -5018,7 +5011,7 @@
         <v>Red</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C75" s="13">
         <v>73</v>
@@ -5033,7 +5026,7 @@
         <v>55</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H75" s="13"/>
       <c r="I75" s="25">
@@ -5055,7 +5048,7 @@
         <v>Red</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C76" s="24">
         <v>74</v>
@@ -5070,7 +5063,7 @@
         <v>55</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H76" s="13"/>
       <c r="I76" s="25">
@@ -5092,7 +5085,7 @@
         <v>Red</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C77" s="13">
         <v>75</v>
@@ -5107,7 +5100,7 @@
         <v>55</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H77" s="13"/>
       <c r="I77" s="25">
@@ -5129,7 +5122,7 @@
         <v>Red</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C78" s="13">
         <v>76</v>
@@ -5144,7 +5137,7 @@
         <v>55</v>
       </c>
       <c r="G78" s="22" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H78" s="13"/>
       <c r="I78" s="25">
@@ -5162,7 +5155,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B79" s="13"/>
       <c r="C79" s="24"/>
@@ -5196,7 +5189,7 @@
       </c>
       <c r="B81" s="13"/>
       <c r="C81" s="24"/>
-      <c r="D81" s="32"/>
+      <c r="D81" s="31"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="str">
@@ -5800,9 +5793,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L58" sqref="L58"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G58" sqref="G58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5852,7 +5845,7 @@
         <v>11</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="L1" s="14"/>
       <c r="M1" s="14"/>
@@ -5871,7 +5864,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="6"/>
@@ -5882,7 +5875,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>13</v>
@@ -5937,10 +5930,10 @@
         <v>45</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I4" s="13">
         <f t="shared" ref="I4:I67" si="0">E4*D4/100</f>
@@ -6182,7 +6175,7 @@
       </c>
       <c r="L10" s="14"/>
       <c r="M10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -6206,10 +6199,10 @@
         <v>45</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="0"/>
@@ -6225,7 +6218,7 @@
       </c>
       <c r="L11" s="14"/>
       <c r="M11" s="18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -6264,7 +6257,7 @@
       </c>
       <c r="L12" s="14"/>
       <c r="M12" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -6347,7 +6340,7 @@
         <v>Green</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="13">
         <v>13</v>
@@ -6362,7 +6355,7 @@
         <v>70</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H15" s="13"/>
       <c r="I15" s="13">
@@ -6386,7 +6379,7 @@
         <v>Green</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="13">
         <v>14</v>
@@ -6423,7 +6416,7 @@
         <v>Green</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="24">
         <v>15</v>
@@ -6458,7 +6451,7 @@
         <v>Green</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="13">
         <v>16</v>
@@ -6473,10 +6466,10 @@
         <v>70</v>
       </c>
       <c r="G18" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I18" s="13">
         <f t="shared" si="0"/>
@@ -6497,7 +6490,7 @@
         <v>Green</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="24">
         <v>17</v>
@@ -6532,7 +6525,7 @@
         <v>Green</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="13">
         <v>18</v>
@@ -6567,7 +6560,7 @@
         <v>Green</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="13">
         <v>19</v>
@@ -6582,7 +6575,7 @@
         <v>60</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H21" s="13"/>
       <c r="I21" s="13">
@@ -6604,7 +6597,7 @@
         <v>Green</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="24">
         <v>20</v>
@@ -6639,7 +6632,7 @@
         <v>Green</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C23" s="13">
         <v>21</v>
@@ -6674,7 +6667,7 @@
         <v>Green</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C24" s="24">
         <v>22</v>
@@ -6689,10 +6682,10 @@
         <v>70</v>
       </c>
       <c r="G24" s="19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I24" s="13">
         <f t="shared" si="0"/>
@@ -6713,7 +6706,7 @@
         <v>Green</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="13">
         <v>23</v>
@@ -6748,7 +6741,7 @@
         <v>Green</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="13">
         <v>24</v>
@@ -6783,7 +6776,7 @@
         <v>Green</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="24">
         <v>25</v>
@@ -6818,7 +6811,7 @@
         <v>Green</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" s="13">
         <v>26</v>
@@ -6853,7 +6846,7 @@
         <v>Green</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="24">
         <v>27</v>
@@ -6888,7 +6881,7 @@
         <v>Green</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C30" s="13">
         <v>28</v>
@@ -6903,7 +6896,7 @@
         <v>30</v>
       </c>
       <c r="G30" s="21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H30" s="13"/>
       <c r="I30" s="13">
@@ -6925,7 +6918,7 @@
         <v>Green</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31" s="13">
         <v>29</v>
@@ -6960,7 +6953,7 @@
         <v>Green</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32" s="24">
         <v>30</v>
@@ -6995,7 +6988,7 @@
         <v>Green</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C33" s="13">
         <v>31</v>
@@ -7010,10 +7003,10 @@
         <v>30</v>
       </c>
       <c r="G33" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I33" s="13">
         <f t="shared" si="0"/>
@@ -7034,7 +7027,7 @@
         <v>Green</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C34" s="24">
         <v>32</v>
@@ -7069,7 +7062,7 @@
         <v>Green</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C35" s="13">
         <v>33</v>
@@ -7104,7 +7097,7 @@
         <v>Green</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" s="13">
         <v>34</v>
@@ -7139,7 +7132,7 @@
         <v>Green</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="24">
         <v>35</v>
@@ -7174,7 +7167,7 @@
         <v>Green</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C38" s="13">
         <v>36</v>
@@ -7189,7 +7182,7 @@
         <v>30</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H38" s="13"/>
       <c r="I38" s="13">
@@ -7211,7 +7204,7 @@
         <v>Green</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C39" s="13">
         <v>37</v>
@@ -7226,7 +7219,7 @@
         <v>30</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H39" s="13"/>
       <c r="I39" s="13">
@@ -7248,7 +7241,7 @@
         <v>Green</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C40" s="24">
         <v>38</v>
@@ -7263,7 +7256,7 @@
         <v>30</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13">
@@ -7285,7 +7278,7 @@
         <v>Green</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C41" s="13">
         <v>39</v>
@@ -7299,11 +7292,11 @@
       <c r="F41" s="13">
         <v>30</v>
       </c>
-      <c r="G41" s="30" t="s">
-        <v>93</v>
+      <c r="G41" s="35" t="s">
+        <v>94</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I41" s="13">
         <f t="shared" si="0"/>
@@ -7324,7 +7317,7 @@
         <v>Green</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C42" s="13">
         <v>40</v>
@@ -7339,7 +7332,7 @@
         <v>30</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H42" s="13"/>
       <c r="I42" s="13">
@@ -7361,7 +7354,7 @@
         <v>Green</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C43" s="24">
         <v>41</v>
@@ -7376,7 +7369,7 @@
         <v>30</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H43" s="13"/>
       <c r="I43" s="13">
@@ -7398,7 +7391,7 @@
         <v>Green</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C44" s="13">
         <v>42</v>
@@ -7413,7 +7406,7 @@
         <v>30</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H44" s="13"/>
       <c r="I44" s="13">
@@ -7435,7 +7428,7 @@
         <v>Green</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C45" s="13">
         <v>43</v>
@@ -7450,7 +7443,7 @@
         <v>30</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H45" s="13"/>
       <c r="I45" s="13">
@@ -7472,7 +7465,7 @@
         <v>Green</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C46" s="24">
         <v>44</v>
@@ -7487,7 +7480,7 @@
         <v>30</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H46" s="13"/>
       <c r="I46" s="13">
@@ -7509,7 +7502,7 @@
         <v>Green</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C47" s="13">
         <v>45</v>
@@ -7524,7 +7517,7 @@
         <v>30</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H47" s="13"/>
       <c r="I47" s="13">
@@ -7546,7 +7539,7 @@
         <v>Green</v>
       </c>
       <c r="B48" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C48" s="13">
         <v>46</v>
@@ -7561,7 +7554,7 @@
         <v>30</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H48" s="13"/>
       <c r="I48" s="13">
@@ -7583,7 +7576,7 @@
         <v>Green</v>
       </c>
       <c r="B49" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C49" s="24">
         <v>47</v>
@@ -7598,7 +7591,7 @@
         <v>30</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H49" s="13"/>
       <c r="I49" s="13">
@@ -7620,7 +7613,7 @@
         <v>Green</v>
       </c>
       <c r="B50" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C50" s="13">
         <v>48</v>
@@ -7634,11 +7627,11 @@
       <c r="F50" s="13">
         <v>30</v>
       </c>
-      <c r="G50" s="30" t="s">
-        <v>94</v>
+      <c r="G50" s="35" t="s">
+        <v>95</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I50" s="13">
         <f t="shared" si="0"/>
@@ -7659,7 +7652,7 @@
         <v>Green</v>
       </c>
       <c r="B51" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C51" s="13">
         <v>49</v>
@@ -7674,7 +7667,7 @@
         <v>30</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H51" s="13"/>
       <c r="I51" s="13">
@@ -7696,7 +7689,7 @@
         <v>Green</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C52" s="24">
         <v>50</v>
@@ -7711,7 +7704,7 @@
         <v>30</v>
       </c>
       <c r="G52" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H52" s="13"/>
       <c r="I52" s="13">
@@ -7733,7 +7726,7 @@
         <v>Green</v>
       </c>
       <c r="B53" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C53" s="13">
         <v>51</v>
@@ -7748,7 +7741,7 @@
         <v>30</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H53" s="13"/>
       <c r="I53" s="13">
@@ -7770,7 +7763,7 @@
         <v>Green</v>
       </c>
       <c r="B54" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C54" s="13">
         <v>52</v>
@@ -7785,7 +7778,7 @@
         <v>30</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H54" s="13"/>
       <c r="I54" s="13">
@@ -7807,7 +7800,7 @@
         <v>Green</v>
       </c>
       <c r="B55" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C55" s="24">
         <v>53</v>
@@ -7822,7 +7815,7 @@
         <v>30</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H55" s="13"/>
       <c r="I55" s="13">
@@ -7844,7 +7837,7 @@
         <v>Green</v>
       </c>
       <c r="B56" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C56" s="13">
         <v>54</v>
@@ -7859,7 +7852,7 @@
         <v>30</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H56" s="13"/>
       <c r="I56" s="13">
@@ -7881,7 +7874,7 @@
         <v>Green</v>
       </c>
       <c r="B57" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C57" s="13">
         <v>55</v>
@@ -7896,7 +7889,7 @@
         <v>30</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H57" s="13"/>
       <c r="I57" s="13">
@@ -7918,7 +7911,7 @@
         <v>Green</v>
       </c>
       <c r="B58" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C58" s="24">
         <v>56</v>
@@ -7932,11 +7925,11 @@
       <c r="F58" s="13">
         <v>30</v>
       </c>
-      <c r="G58" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="H58" s="35" t="s">
-        <v>74</v>
+      <c r="G58" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="H58" s="34" t="s">
+        <v>72</v>
       </c>
       <c r="I58" s="13">
         <f t="shared" si="0"/>
@@ -7957,7 +7950,7 @@
         <v>Green</v>
       </c>
       <c r="B59" s="13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C59" s="13">
         <v>57</v>
@@ -7972,10 +7965,10 @@
         <v>30</v>
       </c>
       <c r="G59" s="21" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I59" s="13">
         <f t="shared" si="0"/>
@@ -7996,7 +7989,7 @@
         <v>Green</v>
       </c>
       <c r="B60" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C60" s="13">
         <v>58</v>
@@ -8031,7 +8024,7 @@
         <v>Green</v>
       </c>
       <c r="B61" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C61" s="24">
         <v>59</v>
@@ -8066,7 +8059,7 @@
         <v>Green</v>
       </c>
       <c r="B62" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C62" s="13">
         <v>60</v>
@@ -8101,7 +8094,7 @@
         <v>Green</v>
       </c>
       <c r="B63" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C63" s="13">
         <v>61</v>
@@ -8136,7 +8129,7 @@
         <v>Green</v>
       </c>
       <c r="B64" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C64" s="24">
         <v>62</v>
@@ -8171,7 +8164,7 @@
         <v>Green</v>
       </c>
       <c r="B65" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C65" s="13">
         <v>63</v>
@@ -8186,7 +8179,7 @@
         <v>70</v>
       </c>
       <c r="G65" s="21" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H65" s="13"/>
       <c r="I65" s="13">
@@ -8208,7 +8201,7 @@
         <v>Green</v>
       </c>
       <c r="B66" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C66" s="13">
         <v>64</v>
@@ -8243,7 +8236,7 @@
         <v>Green</v>
       </c>
       <c r="B67" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C67" s="24">
         <v>65</v>
@@ -8258,10 +8251,10 @@
         <v>70</v>
       </c>
       <c r="G67" s="19" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I67" s="13">
         <f t="shared" si="0"/>
@@ -8282,7 +8275,7 @@
         <v>Green</v>
       </c>
       <c r="B68" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C68" s="13">
         <v>66</v>
@@ -8317,7 +8310,7 @@
         <v>Green</v>
       </c>
       <c r="B69" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C69" s="13">
         <v>67</v>
@@ -8352,7 +8345,7 @@
         <v>Green</v>
       </c>
       <c r="B70" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C70" s="24">
         <v>68</v>
@@ -8387,7 +8380,7 @@
         <v>Green</v>
       </c>
       <c r="B71" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C71" s="13">
         <v>69</v>
@@ -8422,7 +8415,7 @@
         <v>Green</v>
       </c>
       <c r="B72" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C72" s="13">
         <v>70</v>
@@ -8457,7 +8450,7 @@
         <v>Green</v>
       </c>
       <c r="B73" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C73" s="24">
         <v>71</v>
@@ -8492,7 +8485,7 @@
         <v>Green</v>
       </c>
       <c r="B74" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C74" s="13">
         <v>72</v>
@@ -8527,7 +8520,7 @@
         <v>Green</v>
       </c>
       <c r="B75" s="13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C75" s="13">
         <v>73</v>
@@ -8542,10 +8535,10 @@
         <v>40</v>
       </c>
       <c r="G75" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I75" s="13">
         <f t="shared" si="5"/>
@@ -8566,7 +8559,7 @@
         <v>Green</v>
       </c>
       <c r="B76" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C76" s="24">
         <v>74</v>
@@ -8601,7 +8594,7 @@
         <v>Green</v>
       </c>
       <c r="B77" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C77" s="13">
         <v>75</v>
@@ -8636,7 +8629,7 @@
         <v>Green</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C78" s="13">
         <v>76</v>
@@ -8671,7 +8664,7 @@
         <v>Green</v>
       </c>
       <c r="B79" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C79" s="13">
         <v>77</v>
@@ -8686,7 +8679,7 @@
         <v>70</v>
       </c>
       <c r="G79" s="21" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H79" s="13"/>
       <c r="I79" s="13">
@@ -8708,7 +8701,7 @@
         <v>Green</v>
       </c>
       <c r="B80" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C80" s="24">
         <v>78</v>
@@ -8723,10 +8716,10 @@
         <v>70</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I80" s="13">
         <f t="shared" si="8"/>
@@ -8747,7 +8740,7 @@
         <v>Green</v>
       </c>
       <c r="B81" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C81" s="13">
         <v>79</v>
@@ -8782,7 +8775,7 @@
         <v>Green</v>
       </c>
       <c r="B82" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C82" s="13">
         <v>80</v>
@@ -8817,7 +8810,7 @@
         <v>Green</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C83" s="13">
         <v>81</v>
@@ -8852,7 +8845,7 @@
         <v>Green</v>
       </c>
       <c r="B84" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C84" s="24">
         <v>82</v>
@@ -8887,7 +8880,7 @@
         <v>Green</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C85" s="13">
         <v>83</v>
@@ -8922,7 +8915,7 @@
         <v>Green</v>
       </c>
       <c r="B86" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C86" s="13">
         <v>84</v>
@@ -8957,7 +8950,7 @@
         <v>Green</v>
       </c>
       <c r="B87" s="13" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C87" s="13">
         <v>85</v>
@@ -8972,7 +8965,7 @@
         <v>70</v>
       </c>
       <c r="G87" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H87" s="13"/>
       <c r="I87" s="13">
@@ -8994,7 +8987,7 @@
         <v>Green</v>
       </c>
       <c r="B88" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C88" s="24">
         <v>86</v>
@@ -9029,7 +9022,7 @@
         <v>Green</v>
       </c>
       <c r="B89" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C89" s="13">
         <v>87</v>
@@ -9064,7 +9057,7 @@
         <v>Green</v>
       </c>
       <c r="B90" s="13" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C90" s="13">
         <v>88</v>
@@ -9079,10 +9072,10 @@
         <v>25</v>
       </c>
       <c r="G90" s="19" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I90" s="13">
         <f t="shared" si="8"/>
@@ -9103,7 +9096,7 @@
         <v>Green</v>
       </c>
       <c r="B91" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C91" s="13">
         <v>89</v>
@@ -9138,7 +9131,7 @@
         <v>Green</v>
       </c>
       <c r="B92" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C92" s="24">
         <v>90</v>
@@ -9173,7 +9166,7 @@
         <v>Green</v>
       </c>
       <c r="B93" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C93" s="13">
         <v>91</v>
@@ -9208,7 +9201,7 @@
         <v>Green</v>
       </c>
       <c r="B94" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C94" s="13">
         <v>92</v>
@@ -9243,7 +9236,7 @@
         <v>Green</v>
       </c>
       <c r="B95" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C95" s="13">
         <v>93</v>
@@ -9278,7 +9271,7 @@
         <v>Green</v>
       </c>
       <c r="B96" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C96" s="24">
         <v>94</v>
@@ -9313,7 +9306,7 @@
         <v>Green</v>
       </c>
       <c r="B97" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C97" s="13">
         <v>95</v>
@@ -9348,7 +9341,7 @@
         <v>Green</v>
       </c>
       <c r="B98" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C98" s="13">
         <v>96</v>
@@ -9362,11 +9355,11 @@
       <c r="F98" s="13">
         <v>25</v>
       </c>
-      <c r="G98" s="19" t="s">
-        <v>83</v>
+      <c r="G98" s="35" t="s">
+        <v>93</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I98" s="13">
         <f t="shared" si="8"/>
@@ -9387,7 +9380,7 @@
         <v>Green</v>
       </c>
       <c r="B99" s="13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C99" s="13">
         <v>97</v>
@@ -9422,7 +9415,7 @@
         <v>Green</v>
       </c>
       <c r="B100" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C100" s="24">
         <v>98</v>
@@ -9457,7 +9450,7 @@
         <v>Green</v>
       </c>
       <c r="B101" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C101" s="13">
         <v>99</v>
@@ -9492,7 +9485,7 @@
         <v>Green</v>
       </c>
       <c r="B102" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C102" s="13">
         <v>100</v>
@@ -9527,7 +9520,7 @@
         <v>Green</v>
       </c>
       <c r="B103" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C103" s="13">
         <v>101</v>
@@ -9562,7 +9555,7 @@
         <v>Green</v>
       </c>
       <c r="B104" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C104" s="24">
         <v>102</v>
@@ -9597,7 +9590,7 @@
         <v>Green</v>
       </c>
       <c r="B105" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C105" s="13">
         <v>103</v>
@@ -9632,7 +9625,7 @@
         <v>Green</v>
       </c>
       <c r="B106" s="13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C106" s="13">
         <v>104</v>
@@ -9667,7 +9660,7 @@
         <v>Green</v>
       </c>
       <c r="B107" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C107" s="13">
         <v>105</v>
@@ -9686,7 +9679,7 @@
         <v>STATION; DORMONT</v>
       </c>
       <c r="H107" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I107" s="13">
         <f t="shared" si="8"/>
@@ -9707,7 +9700,7 @@
         <v>Green</v>
       </c>
       <c r="B108" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C108" s="24">
         <v>106</v>
@@ -9742,7 +9735,7 @@
         <v>Green</v>
       </c>
       <c r="B109" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C109" s="13">
         <v>107</v>
@@ -9777,7 +9770,7 @@
         <v>Green</v>
       </c>
       <c r="B110" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C110" s="13">
         <v>108</v>
@@ -9812,7 +9805,7 @@
         <v>Green</v>
       </c>
       <c r="B111" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C111" s="13">
         <v>109</v>
@@ -9847,7 +9840,7 @@
         <v>Green</v>
       </c>
       <c r="B112" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C112" s="24">
         <v>110</v>
@@ -9882,7 +9875,7 @@
         <v>Green</v>
       </c>
       <c r="B113" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C113" s="13">
         <v>111</v>
@@ -9917,7 +9910,7 @@
         <v>Green</v>
       </c>
       <c r="B114" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C114" s="13">
         <v>112</v>
@@ -9952,7 +9945,7 @@
         <v>Green</v>
       </c>
       <c r="B115" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C115" s="13">
         <v>113</v>
@@ -9987,7 +9980,7 @@
         <v>Green</v>
       </c>
       <c r="B116" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C116" s="24">
         <v>114</v>
@@ -10007,7 +10000,7 @@
         <v>STATION; GLENBURY</v>
       </c>
       <c r="H116" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I116" s="13">
         <f t="shared" si="10"/>
@@ -10028,7 +10021,7 @@
         <v>Green</v>
       </c>
       <c r="B117" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C117" s="13">
         <v>115</v>
@@ -10063,7 +10056,7 @@
         <v>Green</v>
       </c>
       <c r="B118" s="13" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C118" s="13">
         <v>116</v>
@@ -10098,7 +10091,7 @@
         <v>Green</v>
       </c>
       <c r="B119" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C119" s="13">
         <v>117</v>
@@ -10133,7 +10126,7 @@
         <v>Green</v>
       </c>
       <c r="B120" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C120" s="24">
         <v>118</v>
@@ -10168,7 +10161,7 @@
         <v>Green</v>
       </c>
       <c r="B121" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C121" s="13">
         <v>119</v>
@@ -10203,7 +10196,7 @@
         <v>Green</v>
       </c>
       <c r="B122" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C122" s="13">
         <v>120</v>
@@ -10238,7 +10231,7 @@
         <v>Green</v>
       </c>
       <c r="B123" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C123" s="13">
         <v>121</v>
@@ -10273,7 +10266,7 @@
         <v>Green</v>
       </c>
       <c r="B124" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C124" s="24">
         <v>122</v>
@@ -10288,7 +10281,7 @@
         <v>20</v>
       </c>
       <c r="G124" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H124" s="13"/>
       <c r="I124" s="13">
@@ -10310,7 +10303,7 @@
         <v>Green</v>
       </c>
       <c r="B125" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C125" s="13">
         <v>123</v>
@@ -10326,10 +10319,10 @@
       </c>
       <c r="G125" s="19" t="str">
         <f>G58</f>
-        <v xml:space="preserve">UNDERGROUND; STATION; OVERBROOK; </v>
+        <v>UNDERGROUND; STATION; OVERBROOK</v>
       </c>
       <c r="H125" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I125" s="13">
         <f t="shared" si="10"/>
@@ -10350,7 +10343,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C126" s="13">
         <v>124</v>
@@ -10365,7 +10358,7 @@
         <v>20</v>
       </c>
       <c r="G126" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H126" s="13"/>
       <c r="I126" s="13">
@@ -10387,7 +10380,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C127" s="13">
         <v>125</v>
@@ -10402,7 +10395,7 @@
         <v>20</v>
       </c>
       <c r="G127" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H127" s="13"/>
       <c r="I127" s="13">
@@ -10424,7 +10417,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C128" s="24">
         <v>126</v>
@@ -10439,7 +10432,7 @@
         <v>20</v>
       </c>
       <c r="G128" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H128" s="13"/>
       <c r="I128" s="13">
@@ -10461,7 +10454,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C129" s="13">
         <v>127</v>
@@ -10476,7 +10469,7 @@
         <v>20</v>
       </c>
       <c r="G129" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H129" s="13"/>
       <c r="I129" s="13">
@@ -10498,7 +10491,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C130" s="13">
         <v>128</v>
@@ -10513,7 +10506,7 @@
         <v>20</v>
       </c>
       <c r="G130" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H130" s="13"/>
       <c r="I130" s="13">
@@ -10535,7 +10528,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C131" s="13">
         <v>129</v>
@@ -10550,7 +10543,7 @@
         <v>20</v>
       </c>
       <c r="G131" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H131" s="13"/>
       <c r="I131" s="13">
@@ -10572,7 +10565,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C132" s="24">
         <v>130</v>
@@ -10587,7 +10580,7 @@
         <v>20</v>
       </c>
       <c r="G132" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H132" s="13"/>
       <c r="I132" s="13">
@@ -10609,7 +10602,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C133" s="13">
         <v>131</v>
@@ -10624,7 +10617,7 @@
         <v>20</v>
       </c>
       <c r="G133" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H133" s="13"/>
       <c r="I133" s="13">
@@ -10646,7 +10639,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C134" s="13">
         <v>132</v>
@@ -10662,10 +10655,10 @@
       </c>
       <c r="G134" s="19" t="str">
         <f>G50</f>
-        <v xml:space="preserve">UNDERGROUND; STATION; INGLEWOOD; </v>
+        <v>UNDERGROUND; STATION; INGLEWOOD</v>
       </c>
       <c r="H134" s="13" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I134" s="13">
         <f t="shared" si="10"/>
@@ -10686,7 +10679,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C135" s="13">
         <v>133</v>
@@ -10701,7 +10694,7 @@
         <v>20</v>
       </c>
       <c r="G135" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H135" s="13"/>
       <c r="I135" s="13">
@@ -10723,7 +10716,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C136" s="24">
         <v>134</v>
@@ -10738,7 +10731,7 @@
         <v>20</v>
       </c>
       <c r="G136" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H136" s="13"/>
       <c r="I136" s="13">
@@ -10760,7 +10753,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C137" s="13">
         <v>135</v>
@@ -10775,7 +10768,7 @@
         <v>20</v>
       </c>
       <c r="G137" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H137" s="13"/>
       <c r="I137" s="13">
@@ -10797,7 +10790,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C138" s="13">
         <v>136</v>
@@ -10812,7 +10805,7 @@
         <v>20</v>
       </c>
       <c r="G138" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H138" s="13"/>
       <c r="I138" s="13">
@@ -10834,7 +10827,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C139" s="13">
         <v>137</v>
@@ -10849,7 +10842,7 @@
         <v>20</v>
       </c>
       <c r="G139" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H139" s="13"/>
       <c r="I139" s="13">
@@ -10871,7 +10864,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C140" s="24">
         <v>138</v>
@@ -10886,7 +10879,7 @@
         <v>20</v>
       </c>
       <c r="G140" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H140" s="13"/>
       <c r="I140" s="13">
@@ -10908,7 +10901,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C141" s="13">
         <v>139</v>
@@ -10923,7 +10916,7 @@
         <v>20</v>
       </c>
       <c r="G141" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H141" s="13"/>
       <c r="I141" s="13">
@@ -10945,7 +10938,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C142" s="13">
         <v>140</v>
@@ -10960,7 +10953,7 @@
         <v>20</v>
       </c>
       <c r="G142" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H142" s="13"/>
       <c r="I142" s="13">
@@ -10982,7 +10975,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C143" s="13">
         <v>141</v>
@@ -10998,10 +10991,10 @@
       </c>
       <c r="G143" s="19" t="str">
         <f>G41</f>
-        <v xml:space="preserve">UNDERGROUND; STATION; CENTRAL; </v>
+        <v>UNDERGROUND; STATION; CENTRAL</v>
       </c>
       <c r="H143" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I143" s="13">
         <f t="shared" si="10"/>
@@ -11022,7 +11015,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C144" s="24">
         <v>142</v>
@@ -11037,7 +11030,7 @@
         <v>20</v>
       </c>
       <c r="G144" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H144" s="13"/>
       <c r="I144" s="13">
@@ -11059,7 +11052,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C145" s="13">
         <v>143</v>
@@ -11074,7 +11067,7 @@
         <v>20</v>
       </c>
       <c r="G145" s="13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H145" s="13"/>
       <c r="I145" s="13">
@@ -11096,7 +11089,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C146" s="13">
         <v>144</v>
@@ -11131,7 +11124,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C147" s="13">
         <v>145</v>
@@ -11166,7 +11159,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C148" s="24">
         <v>146</v>
@@ -11201,7 +11194,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C149" s="13">
         <v>147</v>
@@ -11236,7 +11229,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C150" s="13">
         <v>148</v>
@@ -11272,7 +11265,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C151" s="13">
         <v>149</v>
@@ -11307,7 +11300,7 @@
         <v>Green</v>
       </c>
       <c r="B152" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C152" s="24">
         <v>150</v>
@@ -11388,34 +11381,34 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="F1" s="34"/>
-      <c r="G1" s="34"/>
-      <c r="H1" s="34"/>
-      <c r="I1" s="34"/>
-      <c r="J1" s="34"/>
+      <c r="A1" s="33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
+      <c r="A2" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="E8" s="8"/>

</xml_diff>